<commit_message>
Update QA Tests Table
</commit_message>
<xml_diff>
--- a/Documentation & Presentation/QA Tests Table.xlsx
+++ b/Documentation & Presentation/QA Tests Table.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks\Documents\GitHub\Maze-Project\Documentation &amp; Presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6EA7523-8DA8-4991-A1F6-73A9DFAD3E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FBE01A-C2D7-46DB-BE28-BD23B70C193F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="599" xr2:uid="{A330392C-FB42-43E4-881D-7EBDC550B0C9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="599" activeTab="3" xr2:uid="{A330392C-FB42-43E4-881D-7EBDC550B0C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Suite 1" sheetId="1" r:id="rId1"/>
     <sheet name="Test Suite 2" sheetId="3" r:id="rId2"/>
+    <sheet name="Test Suite 3" sheetId="4" r:id="rId3"/>
+    <sheet name="Test Suite 4" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="110">
   <si>
     <t xml:space="preserve">Main Menu </t>
   </si>
@@ -124,9 +126,6 @@
     <t>Esc</t>
   </si>
   <si>
-    <t>To quit the main menu</t>
-  </si>
-  <si>
     <t>T_002</t>
   </si>
   <si>
@@ -136,15 +135,9 @@
     <t>Main Menu Display</t>
   </si>
   <si>
-    <t>Main Menu Start Option</t>
-  </si>
-  <si>
     <t>Navigating to and entering the first option</t>
   </si>
   <si>
-    <t>Testing if the program successfully enters the starting option</t>
-  </si>
-  <si>
     <t>To display "select level" and options</t>
   </si>
   <si>
@@ -233,6 +226,147 @@
   </si>
   <si>
     <t>Navigating to and entering the third option</t>
+  </si>
+  <si>
+    <t>Displaying heading and levels</t>
+  </si>
+  <si>
+    <t>To quit the program and print "see you soon"</t>
+  </si>
+  <si>
+    <t>T_012</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Start Options Active Color Change</t>
+  </si>
+  <si>
+    <t>Entering level easy</t>
+  </si>
+  <si>
+    <t>To display a 10x10 maze</t>
+  </si>
+  <si>
+    <t>T_013</t>
+  </si>
+  <si>
+    <t>T_014</t>
+  </si>
+  <si>
+    <t>Testing if the program displays the maze of medium difficulty properly</t>
+  </si>
+  <si>
+    <t>Testing if the program displays the maze of easy difficulty properly</t>
+  </si>
+  <si>
+    <t>Testing if the program displays the maze of hard difficulty properly</t>
+  </si>
+  <si>
+    <t>Entering level medium</t>
+  </si>
+  <si>
+    <t>To display a 15x15 maze</t>
+  </si>
+  <si>
+    <t>To display a 20x20 maze</t>
+  </si>
+  <si>
+    <t>Entering level hard</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Start Options Easy Maze</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Start Options Medium Maze</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Start Options Hard Maze</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Start Options Easy Keys</t>
+  </si>
+  <si>
+    <t>To randomly display 2 keys in places with 3 walls</t>
+  </si>
+  <si>
+    <t>T_015</t>
+  </si>
+  <si>
+    <t>TEST CASE 6</t>
+  </si>
+  <si>
+    <t>T_016</t>
+  </si>
+  <si>
+    <t>Testing if the program displays the keys in easy maze properly</t>
+  </si>
+  <si>
+    <t>Testing if the program displays the keys in medium maze properly</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Start Options Medium Keys</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Start Options Hard Keys</t>
+  </si>
+  <si>
+    <t>To randomly display 4 keys in places with 3 walls</t>
+  </si>
+  <si>
+    <t>To randomly display 8 keys in places with 3 walls</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Start Options Go Back</t>
+  </si>
+  <si>
+    <t>Entering option Go Back</t>
+  </si>
+  <si>
+    <t>To return to main menu</t>
+  </si>
+  <si>
+    <t>Testing if the program return to main menu from the starting options</t>
+  </si>
+  <si>
+    <t>T_021</t>
+  </si>
+  <si>
+    <t>Leaderboard Display</t>
+  </si>
+  <si>
+    <t>Displaying best scores according to difficulty</t>
+  </si>
+  <si>
+    <t>To display all high scores</t>
+  </si>
+  <si>
+    <t>Returning to Main Menu</t>
+  </si>
+  <si>
+    <t>To return to the main menu</t>
+  </si>
+  <si>
+    <t>Testing if the program displays heading and best scores properly of leaderboard tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leaderboard </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rules </t>
+  </si>
+  <si>
+    <t>T_031</t>
+  </si>
+  <si>
+    <t>Testing if the program displays heading and rules of the tab "Rules"</t>
+  </si>
+  <si>
+    <t>Rules Display</t>
+  </si>
+  <si>
+    <t>Displaying rules text</t>
+  </si>
+  <si>
+    <t>To display the rules</t>
   </si>
 </sst>
 </file>
@@ -243,7 +377,7 @@
     <numFmt numFmtId="164" formatCode="[$-2000000]h:mm:ss;@"/>
     <numFmt numFmtId="165" formatCode="dd/m/yyyy\ h:mm"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,6 +440,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -499,7 +641,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -604,6 +746,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -926,8 +1089,8 @@
   </sheetPr>
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1021,7 +1184,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="15"/>
@@ -1166,7 +1329,7 @@
         <v>28</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="1" t="s">
@@ -1179,7 +1342,7 @@
     <row r="20" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="30" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B21" s="30"/>
       <c r="C21" s="30"/>
@@ -1216,7 +1379,7 @@
         <v>2</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="15"/>
@@ -1234,7 +1397,7 @@
         <v>5</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C26" s="14"/>
       <c r="D26" s="15"/>
@@ -1252,7 +1415,7 @@
         <v>7</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C27" s="22"/>
       <c r="D27" s="23"/>
@@ -1274,7 +1437,7 @@
         <v>9</v>
       </c>
       <c r="F28" s="16">
-        <v>44508.93888883102</v>
+        <v>44508.650694444441</v>
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="18"/>
@@ -1328,14 +1491,14 @@
         <v>2</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="1" t="s">
@@ -1350,14 +1513,14 @@
         <v>3</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="1" t="s">
@@ -1379,7 +1542,7 @@
         <v>28</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F34" s="8"/>
       <c r="G34" s="1" t="s">
@@ -1392,7 +1555,7 @@
     <row r="36" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="30" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B37" s="30"/>
       <c r="C37" s="30"/>
@@ -1429,7 +1592,7 @@
         <v>2</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C41" s="14"/>
       <c r="D41" s="15"/>
@@ -1447,7 +1610,7 @@
         <v>5</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C42" s="14"/>
       <c r="D42" s="15"/>
@@ -1455,7 +1618,7 @@
         <v>6</v>
       </c>
       <c r="F42" s="16">
-        <v>44509.934027777781</v>
+        <v>44509.65347222222</v>
       </c>
       <c r="G42" s="17"/>
       <c r="H42" s="18"/>
@@ -1465,7 +1628,7 @@
         <v>7</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C43" s="22"/>
       <c r="D43" s="23"/>
@@ -1487,7 +1650,7 @@
         <v>9</v>
       </c>
       <c r="F44" s="16">
-        <v>44509.93888883102</v>
+        <v>44509.656944444447</v>
       </c>
       <c r="G44" s="17"/>
       <c r="H44" s="18"/>
@@ -1541,14 +1704,14 @@
         <v>2</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F48" s="8"/>
       <c r="G48" s="1" t="s">
@@ -1570,7 +1733,7 @@
         <v>28</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F49" s="8"/>
       <c r="G49" s="1" t="s">
@@ -1582,7 +1745,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="30" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B52" s="30"/>
       <c r="C52" s="30"/>
@@ -1619,7 +1782,7 @@
         <v>2</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C56" s="14"/>
       <c r="D56" s="15"/>
@@ -1637,7 +1800,7 @@
         <v>5</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C57" s="14"/>
       <c r="D57" s="15"/>
@@ -1645,7 +1808,7 @@
         <v>6</v>
       </c>
       <c r="F57" s="16">
-        <v>44510.934027777781</v>
+        <v>44510.65902777778</v>
       </c>
       <c r="G57" s="17"/>
       <c r="H57" s="18"/>
@@ -1655,7 +1818,7 @@
         <v>7</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C58" s="22"/>
       <c r="D58" s="23"/>
@@ -1677,7 +1840,7 @@
         <v>9</v>
       </c>
       <c r="F59" s="16">
-        <v>44510.93888883102</v>
+        <v>44510.662499999999</v>
       </c>
       <c r="G59" s="17"/>
       <c r="H59" s="18"/>
@@ -1731,14 +1894,14 @@
         <v>2</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F63" s="12"/>
       <c r="G63" s="1" t="s">
@@ -1760,7 +1923,7 @@
         <v>28</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F64" s="8"/>
       <c r="G64" s="1" t="s">
@@ -1772,7 +1935,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="30" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B67" s="30"/>
       <c r="C67" s="30"/>
@@ -1809,7 +1972,7 @@
         <v>2</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C71" s="14"/>
       <c r="D71" s="15"/>
@@ -1827,7 +1990,7 @@
         <v>5</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C72" s="14"/>
       <c r="D72" s="15"/>
@@ -1835,7 +1998,7 @@
         <v>6</v>
       </c>
       <c r="F72" s="16">
-        <v>44511.934027777781</v>
+        <v>44511.663888888892</v>
       </c>
       <c r="G72" s="17"/>
       <c r="H72" s="18"/>
@@ -1845,7 +2008,7 @@
         <v>7</v>
       </c>
       <c r="B73" s="21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C73" s="22"/>
       <c r="D73" s="23"/>
@@ -1867,7 +2030,7 @@
         <v>9</v>
       </c>
       <c r="F74" s="16">
-        <v>44511.93888883102</v>
+        <v>44511.667361111111</v>
       </c>
       <c r="G74" s="17"/>
       <c r="H74" s="18"/>
@@ -1921,14 +2084,14 @@
         <v>2</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C78" s="8"/>
       <c r="D78" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F78" s="12"/>
       <c r="G78" s="1" t="s">
@@ -1950,7 +2113,7 @@
         <v>28</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F79" s="8"/>
       <c r="G79" s="1" t="s">
@@ -2067,17 +2230,17 @@
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H127"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:C16"/>
+    <sheetView topLeftCell="A115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -2146,7 +2309,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="15"/>
@@ -2164,7 +2327,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="15"/>
@@ -2172,7 +2335,7 @@
         <v>6</v>
       </c>
       <c r="F10" s="16">
-        <v>44508.654166666667</v>
+        <v>44508.675000000003</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="18"/>
@@ -2182,7 +2345,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C11" s="22"/>
       <c r="D11" s="23"/>
@@ -2204,7 +2367,7 @@
         <v>9</v>
       </c>
       <c r="F12" s="16">
-        <v>44508.656944444447</v>
+        <v>44508.678472222222</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="18"/>
@@ -2258,14 +2421,14 @@
         <v>2</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="1" t="s">
@@ -2277,17 +2440,17 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="1" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="1" t="s">
@@ -2297,29 +2460,2124 @@
         <v>20</v>
       </c>
     </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>4</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="34"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="14"/>
+      <c r="H25" s="15"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="16">
+        <v>44509.679861111108</v>
+      </c>
+      <c r="G26" s="17"/>
+      <c r="H26" s="18"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="28"/>
+      <c r="H27" s="29"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="20"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="16">
+        <v>44509.682638888888</v>
+      </c>
+      <c r="G28" s="17"/>
+      <c r="H28" s="18"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="10"/>
+      <c r="D30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="10"/>
+      <c r="G30" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>1</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>2</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>3</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F33" s="8"/>
+      <c r="G33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="31"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="34"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="14"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G40" s="14"/>
+      <c r="H40" s="15"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" s="16">
+        <v>44510.693055555559</v>
+      </c>
+      <c r="G41" s="17"/>
+      <c r="H41" s="18"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="22"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="28"/>
+      <c r="H42" s="29"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="20"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="16">
+        <v>44510.696527777778</v>
+      </c>
+      <c r="G43" s="17"/>
+      <c r="H43" s="18"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="10"/>
+      <c r="D45" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" s="10"/>
+      <c r="G45" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>1</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="8"/>
+      <c r="D46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46" s="8"/>
+      <c r="G46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>2</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F47" s="8"/>
+      <c r="G47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>3</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" s="8"/>
+      <c r="D48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F48" s="8"/>
+      <c r="G48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="30"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="30"/>
+      <c r="H51" s="30"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="31"/>
+      <c r="B52" s="31"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="31"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="31"/>
+      <c r="H52" s="31"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" s="33"/>
+      <c r="C54" s="33"/>
+      <c r="D54" s="33"/>
+      <c r="E54" s="33"/>
+      <c r="F54" s="33"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="34"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C55" s="14"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G55" s="14"/>
+      <c r="H55" s="15"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" s="14"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F56" s="16">
+        <v>44510.699305555558</v>
+      </c>
+      <c r="G56" s="17"/>
+      <c r="H56" s="18"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C57" s="22"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G57" s="28"/>
+      <c r="H57" s="29"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="20"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="25"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" s="16">
+        <v>44510.70208333333</v>
+      </c>
+      <c r="G58" s="17"/>
+      <c r="H58" s="18"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="10"/>
+      <c r="D60" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F60" s="10"/>
+      <c r="G60" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
+        <v>1</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" s="8"/>
+      <c r="D61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F61" s="8"/>
+      <c r="G61" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
+        <v>2</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C62" s="8"/>
+      <c r="D62" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F62" s="8"/>
+      <c r="G62" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
+        <v>3</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" s="8"/>
+      <c r="D63" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F63" s="8"/>
+      <c r="G63" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B66" s="30"/>
+      <c r="C66" s="30"/>
+      <c r="D66" s="30"/>
+      <c r="E66" s="30"/>
+      <c r="F66" s="30"/>
+      <c r="G66" s="30"/>
+      <c r="H66" s="30"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67" s="31"/>
+      <c r="B67" s="31"/>
+      <c r="C67" s="31"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="31"/>
+      <c r="F67" s="31"/>
+      <c r="G67" s="31"/>
+      <c r="H67" s="31"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69" s="33"/>
+      <c r="C69" s="33"/>
+      <c r="D69" s="33"/>
+      <c r="E69" s="33"/>
+      <c r="F69" s="33"/>
+      <c r="G69" s="33"/>
+      <c r="H69" s="34"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C70" s="14"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F70" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G70" s="14"/>
+      <c r="H70" s="15"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C71" s="14"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F71" s="16">
+        <v>44511.703472222223</v>
+      </c>
+      <c r="G71" s="17"/>
+      <c r="H71" s="18"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B72" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C72" s="22"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F72" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G72" s="28"/>
+      <c r="H72" s="29"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73" s="20"/>
+      <c r="B73" s="24"/>
+      <c r="C73" s="25"/>
+      <c r="D73" s="26"/>
+      <c r="E73" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73" s="16">
+        <v>44511.705555555556</v>
+      </c>
+      <c r="G73" s="17"/>
+      <c r="H73" s="18"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" s="10"/>
+      <c r="D75" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F75" s="10"/>
+      <c r="G75" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>1</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C76" s="8"/>
+      <c r="D76" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F76" s="8"/>
+      <c r="G76" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
+        <v>2</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C77" s="8"/>
+      <c r="D77" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F77" s="8"/>
+      <c r="G77" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
+        <v>3</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C78" s="8"/>
+      <c r="D78" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F78" s="8"/>
+      <c r="G78" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A81" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B81" s="30"/>
+      <c r="C81" s="30"/>
+      <c r="D81" s="30"/>
+      <c r="E81" s="30"/>
+      <c r="F81" s="30"/>
+      <c r="G81" s="30"/>
+      <c r="H81" s="30"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A82" s="31"/>
+      <c r="B82" s="31"/>
+      <c r="C82" s="31"/>
+      <c r="D82" s="31"/>
+      <c r="E82" s="31"/>
+      <c r="F82" s="31"/>
+      <c r="G82" s="31"/>
+      <c r="H82" s="31"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A84" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B84" s="33"/>
+      <c r="C84" s="33"/>
+      <c r="D84" s="33"/>
+      <c r="E84" s="33"/>
+      <c r="F84" s="33"/>
+      <c r="G84" s="33"/>
+      <c r="H84" s="34"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B85" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C85" s="14"/>
+      <c r="D85" s="15"/>
+      <c r="E85" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F85" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G85" s="14"/>
+      <c r="H85" s="15"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B86" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C86" s="14"/>
+      <c r="D86" s="15"/>
+      <c r="E86" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F86" s="16">
+        <v>44512.706250000003</v>
+      </c>
+      <c r="G86" s="17"/>
+      <c r="H86" s="18"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A87" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B87" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C87" s="22"/>
+      <c r="D87" s="23"/>
+      <c r="E87" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F87" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G87" s="28"/>
+      <c r="H87" s="29"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A88" s="20"/>
+      <c r="B88" s="24"/>
+      <c r="C88" s="25"/>
+      <c r="D88" s="26"/>
+      <c r="E88" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F88" s="16">
+        <v>44512.709027777775</v>
+      </c>
+      <c r="G88" s="17"/>
+      <c r="H88" s="18"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A90" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C90" s="10"/>
+      <c r="D90" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F90" s="10"/>
+      <c r="G90" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A91" s="1">
+        <v>4</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C91" s="8"/>
+      <c r="D91" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F91" s="8"/>
+      <c r="G91" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A92" s="1">
+        <v>5</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C92" s="8"/>
+      <c r="D92" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F92" s="8"/>
+      <c r="G92" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A93" s="1">
+        <v>6</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C93" s="8"/>
+      <c r="D93" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E93" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F93" s="8"/>
+      <c r="G93" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A96" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B96" s="30"/>
+      <c r="C96" s="30"/>
+      <c r="D96" s="30"/>
+      <c r="E96" s="30"/>
+      <c r="F96" s="30"/>
+      <c r="G96" s="30"/>
+      <c r="H96" s="30"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A97" s="31"/>
+      <c r="B97" s="31"/>
+      <c r="C97" s="31"/>
+      <c r="D97" s="31"/>
+      <c r="E97" s="31"/>
+      <c r="F97" s="31"/>
+      <c r="G97" s="31"/>
+      <c r="H97" s="31"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A99" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B99" s="33"/>
+      <c r="C99" s="33"/>
+      <c r="D99" s="33"/>
+      <c r="E99" s="33"/>
+      <c r="F99" s="33"/>
+      <c r="G99" s="33"/>
+      <c r="H99" s="34"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A100" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B100" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C100" s="14"/>
+      <c r="D100" s="15"/>
+      <c r="E100" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F100" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G100" s="14"/>
+      <c r="H100" s="15"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A101" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B101" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C101" s="14"/>
+      <c r="D101" s="15"/>
+      <c r="E101" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F101" s="16">
+        <v>44512.710416666669</v>
+      </c>
+      <c r="G101" s="17"/>
+      <c r="H101" s="18"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A102" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B102" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C102" s="22"/>
+      <c r="D102" s="23"/>
+      <c r="E102" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F102" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G102" s="28"/>
+      <c r="H102" s="29"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A103" s="20"/>
+      <c r="B103" s="24"/>
+      <c r="C103" s="25"/>
+      <c r="D103" s="26"/>
+      <c r="E103" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F103" s="16">
+        <v>44512.713194444441</v>
+      </c>
+      <c r="G103" s="17"/>
+      <c r="H103" s="18"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A105" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105" s="10"/>
+      <c r="D105" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E105" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F105" s="10"/>
+      <c r="G105" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H105" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A106" s="1">
+        <v>4</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C106" s="8"/>
+      <c r="D106" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E106" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F106" s="8"/>
+      <c r="G106" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A107" s="1">
+        <v>5</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C107" s="8"/>
+      <c r="D107" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E107" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F107" s="8"/>
+      <c r="G107" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A108" s="1">
+        <v>6</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C108" s="8"/>
+      <c r="D108" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F108" s="8"/>
+      <c r="G108" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A111" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B111" s="30"/>
+      <c r="C111" s="30"/>
+      <c r="D111" s="30"/>
+      <c r="E111" s="30"/>
+      <c r="F111" s="30"/>
+      <c r="G111" s="30"/>
+      <c r="H111" s="30"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A112" s="31"/>
+      <c r="B112" s="31"/>
+      <c r="C112" s="31"/>
+      <c r="D112" s="31"/>
+      <c r="E112" s="31"/>
+      <c r="F112" s="31"/>
+      <c r="G112" s="31"/>
+      <c r="H112" s="31"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A114" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B114" s="33"/>
+      <c r="C114" s="33"/>
+      <c r="D114" s="33"/>
+      <c r="E114" s="33"/>
+      <c r="F114" s="33"/>
+      <c r="G114" s="33"/>
+      <c r="H114" s="34"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A115" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B115" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C115" s="14"/>
+      <c r="D115" s="15"/>
+      <c r="E115" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F115" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G115" s="14"/>
+      <c r="H115" s="15"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A116" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B116" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C116" s="14"/>
+      <c r="D116" s="15"/>
+      <c r="E116" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F116" s="16">
+        <v>44513.714583333334</v>
+      </c>
+      <c r="G116" s="17"/>
+      <c r="H116" s="18"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A117" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B117" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C117" s="22"/>
+      <c r="D117" s="23"/>
+      <c r="E117" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F117" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G117" s="28"/>
+      <c r="H117" s="29"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A118" s="20"/>
+      <c r="B118" s="24"/>
+      <c r="C118" s="25"/>
+      <c r="D118" s="26"/>
+      <c r="E118" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F118" s="16">
+        <v>44513.717361111114</v>
+      </c>
+      <c r="G118" s="17"/>
+      <c r="H118" s="18"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A120" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B120" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C120" s="10"/>
+      <c r="D120" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E120" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F120" s="10"/>
+      <c r="G120" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H120" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A121" s="1">
+        <v>7</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C121" s="8"/>
+      <c r="D121" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E121" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F121" s="8"/>
+      <c r="G121" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A122" s="1">
+        <v>8</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C122" s="8"/>
+      <c r="D122" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E122" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F122" s="8"/>
+      <c r="G122" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A123" s="1">
+        <v>9</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C123" s="8"/>
+      <c r="D123" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E123" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F123" s="8"/>
+      <c r="G123" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="127" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="A1:H3"/>
-    <mergeCell ref="A5:H6"/>
+  <mergeCells count="147">
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="E90:F90"/>
+    <mergeCell ref="E105:F105"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B122:C122"/>
+    <mergeCell ref="E122:F122"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="E123:F123"/>
+    <mergeCell ref="A117:A118"/>
+    <mergeCell ref="B117:D118"/>
+    <mergeCell ref="F117:H117"/>
+    <mergeCell ref="F118:H118"/>
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="E121:F121"/>
+    <mergeCell ref="E120:F120"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="A114:H114"/>
+    <mergeCell ref="B115:D115"/>
+    <mergeCell ref="F115:H115"/>
+    <mergeCell ref="B116:D116"/>
+    <mergeCell ref="F116:H116"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="E107:F107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="E108:F108"/>
+    <mergeCell ref="A111:H112"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="B102:D103"/>
+    <mergeCell ref="F102:H102"/>
+    <mergeCell ref="F103:H103"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="E106:F106"/>
+    <mergeCell ref="A99:H99"/>
+    <mergeCell ref="B100:D100"/>
+    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="F101:H101"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="E92:F92"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="E93:F93"/>
+    <mergeCell ref="A96:H97"/>
+    <mergeCell ref="A87:A88"/>
+    <mergeCell ref="B87:D88"/>
+    <mergeCell ref="F87:H87"/>
+    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="E91:F91"/>
+    <mergeCell ref="A84:H84"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="F85:H85"/>
+    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="F86:H86"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="A81:H82"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="B72:D73"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="A69:H69"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="A66:H67"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="B57:D58"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="A54:H54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="A51:H52"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:D43"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="A36:H37"/>
+    <mergeCell ref="A39:H39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:D28"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:D12"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="E15:F15"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="F9:H9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="A5:H6"/>
+    <mergeCell ref="A21:H22"/>
+    <mergeCell ref="A1:H3"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E14:F14"/>
+  </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F142FD8-31A4-49BC-9B4D-043E26A06CB3}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="34"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="16">
+        <v>44507.722916666666</v>
+      </c>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="37"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="28"/>
+      <c r="H11" s="29"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="20"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="16">
+        <v>44507.725694444445</v>
+      </c>
+      <c r="G12" s="17"/>
+      <c r="H12" s="18"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>2</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>3</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>4</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>5</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="23">
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:D12"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="E14:F14"/>
+    <mergeCell ref="A1:H3"/>
+    <mergeCell ref="A5:H6"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="F10:H10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8641709E-5E2F-494E-8F93-4F65260E4FD8}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="34"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="16">
+        <v>44507.727777777778</v>
+      </c>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="37"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="28"/>
+      <c r="H11" s="29"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="20"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="16">
+        <v>44507.730555555558</v>
+      </c>
+      <c r="G12" s="17"/>
+      <c r="H12" s="18"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>2</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>3</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>4</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>5</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="23">
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E19:F19"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:D12"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="A1:H3"/>
+    <mergeCell ref="A5:H6"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="F10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>